<commit_message>
Ajuste estilos Beneficios, Disponibilidades, Crews y Home
</commit_message>
<xml_diff>
--- a/Backend/python/Datos_v8.xlsx
+++ b/Backend/python/Datos_v8.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="127">
   <si>
     <t>ID</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>asda</t>
+  </si>
+  <si>
+    <t>adsasddas</t>
   </si>
   <si>
     <t>Hora inicio bloque</t>
@@ -973,13 +976,13 @@
   <sheetData>
     <row r="1" ht="26.25" customHeight="1" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -1088,7 +1091,7 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
@@ -1112,7 +1115,7 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
@@ -1156,7 +1159,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B13" s="29"/>
       <c r="E13" s="21"/>
@@ -1175,18 +1178,18 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B18" s="33">
         <v>1</v>
@@ -1197,7 +1200,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="32" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B19" s="33">
         <v>2</v>
@@ -1208,7 +1211,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="32" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B20" s="33">
         <v>3</v>
@@ -1219,7 +1222,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="32" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B21" s="33">
         <v>4</v>
@@ -1230,7 +1233,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="32" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B22" s="33">
         <v>5</v>
@@ -1241,7 +1244,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="32" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B23" s="33">
         <v>6</v>
@@ -1252,7 +1255,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="32" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B24" s="33">
         <v>7</v>
@@ -1285,37 +1288,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -3151,8 +3154,21 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
       <c r="H21" s="1">
         <v>16</v>
       </c>
@@ -19548,25 +19564,25 @@
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I2" s="35">
         <v>0.3333333333321207</v>
@@ -19668,7 +19684,7 @@
     <row r="3" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -19788,7 +19804,7 @@
     <row r="4" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
@@ -19908,7 +19924,7 @@
     <row r="5" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
@@ -20028,7 +20044,7 @@
     <row r="6" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C6" s="1">
         <v>5</v>
@@ -20148,7 +20164,7 @@
     <row r="7" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C7" s="1">
         <v>7</v>
@@ -20268,7 +20284,7 @@
     <row r="8" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C8" s="1">
         <v>9</v>
@@ -20388,7 +20404,7 @@
     <row r="9" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C9" s="1">
         <v>12</v>
@@ -21097,7 +21113,7 @@
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="38" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -21132,25 +21148,25 @@
         <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I2" s="35">
         <v>0.3333333333321207</v>
@@ -21252,7 +21268,7 @@
     <row r="3" spans="1:40" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="44"/>
       <c r="B3" s="45" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C3" s="46">
         <v>2</v>
@@ -21372,7 +21388,7 @@
     <row r="4" spans="1:40" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="44"/>
       <c r="B4" s="45" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C4" s="46">
         <v>2</v>
@@ -21492,7 +21508,7 @@
     <row r="5" spans="1:40" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="44"/>
       <c r="B5" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C5" s="10">
         <v>3</v>
@@ -21612,7 +21628,7 @@
     <row r="6" spans="1:40" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="44"/>
       <c r="B6" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C6" s="10">
         <v>5</v>
@@ -21732,7 +21748,7 @@
     <row r="7" spans="1:40" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="44"/>
       <c r="B7" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C7" s="10">
         <v>7</v>
@@ -21851,7 +21867,7 @@
     </row>
     <row r="8" spans="2:40" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="45" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C8" s="46">
         <v>9</v>
@@ -21971,7 +21987,7 @@
     <row r="9" spans="1:40" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="44"/>
       <c r="B9" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C9" s="10">
         <v>9</v>
@@ -22090,7 +22106,7 @@
     </row>
     <row r="10" spans="2:40" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="45" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C10" s="46">
         <v>11</v>
@@ -22210,7 +22226,7 @@
     <row r="11" spans="1:40" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="44"/>
       <c r="B11" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C11" s="10">
         <v>11</v>
@@ -22330,7 +22346,7 @@
     <row r="12" spans="1:40" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="44"/>
       <c r="B12" s="45" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C12" s="46">
         <v>11</v>
@@ -22450,7 +22466,7 @@
     <row r="13" spans="1:40" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="44"/>
       <c r="B13" s="45" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C13" s="46">
         <v>13</v>
@@ -22570,7 +22586,7 @@
     <row r="14" spans="1:41" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="44"/>
       <c r="B14" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C14" s="10">
         <v>13</v>
@@ -22691,7 +22707,7 @@
     <row r="15" spans="1:41" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="44"/>
       <c r="B15" s="45" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C15" s="46">
         <v>14</v>
@@ -22812,7 +22828,7 @@
     <row r="16" spans="1:40" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="51"/>
       <c r="B16" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C16" s="10">
         <v>14</v>
@@ -22932,7 +22948,7 @@
     <row r="17" spans="1:40" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="51"/>
       <c r="B17" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C17" s="10">
         <v>15</v>
@@ -23052,7 +23068,7 @@
     <row r="18" spans="1:40" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="51"/>
       <c r="B18" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C18" s="10">
         <v>18</v>
@@ -23172,7 +23188,7 @@
     <row r="19" spans="1:40" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="51"/>
       <c r="B19" s="45" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C19" s="46">
         <v>20</v>
@@ -24232,7 +24248,7 @@
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="38" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -24267,25 +24283,25 @@
         <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I2" s="35">
         <v>0.3333333333321207</v>
@@ -24387,7 +24403,7 @@
     <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" s="34"/>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C3" s="1">
         <v>5</v>
@@ -24507,7 +24523,7 @@
     <row r="4" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="52" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C4" s="53">
         <v>5</v>
@@ -24627,7 +24643,7 @@
     <row r="5" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C5" s="1">
         <v>7</v>
@@ -24747,7 +24763,7 @@
     <row r="6" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C6" s="1">
         <v>9</v>
@@ -24867,7 +24883,7 @@
     <row r="7" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C7" s="1">
         <v>11</v>
@@ -24987,7 +25003,7 @@
     <row r="8" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="52" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C8" s="53">
         <v>13</v>
@@ -25107,7 +25123,7 @@
     <row r="9" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="52" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C9" s="53">
         <v>14</v>
@@ -25227,7 +25243,7 @@
     <row r="10" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C10" s="1">
         <v>13</v>
@@ -25347,7 +25363,7 @@
     <row r="11" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C11" s="1">
         <v>14</v>
@@ -25467,7 +25483,7 @@
     <row r="12" spans="1:40" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="39"/>
       <c r="B12" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C12" s="1">
         <v>15</v>
@@ -25587,7 +25603,7 @@
     <row r="13" spans="1:40" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="39"/>
       <c r="B13" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C13" s="1">
         <v>17</v>
@@ -25707,7 +25723,7 @@
     <row r="14" spans="1:40" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="39"/>
       <c r="B14" s="52" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C14" s="53">
         <v>18</v>
@@ -25827,7 +25843,7 @@
     <row r="15" spans="1:40" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="39"/>
       <c r="B15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C15" s="1">
         <v>20</v>
@@ -26650,7 +26666,7 @@
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="38" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -26685,25 +26701,25 @@
         <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I2" s="35">
         <v>0.3333333333321207</v>
@@ -26804,7 +26820,7 @@
     </row>
     <row r="3" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -26923,7 +26939,7 @@
     </row>
     <row r="4" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B4" s="52" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C4" s="53">
         <v>1</v>
@@ -27042,7 +27058,7 @@
     </row>
     <row r="5" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
@@ -27161,7 +27177,7 @@
     </row>
     <row r="6" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B6" s="52" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C6" s="53">
         <v>2</v>
@@ -27280,7 +27296,7 @@
     </row>
     <row r="7" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B7" s="52" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C7" s="53">
         <v>3</v>
@@ -27399,7 +27415,7 @@
     </row>
     <row r="8" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C8" s="1">
         <v>3</v>
@@ -27518,7 +27534,7 @@
     </row>
     <row r="9" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B9" s="52" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C9" s="53">
         <v>5</v>
@@ -27637,7 +27653,7 @@
     </row>
     <row r="10" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C10" s="1">
         <v>5</v>
@@ -27756,7 +27772,7 @@
     </row>
     <row r="11" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C11" s="1">
         <v>7</v>
@@ -27875,7 +27891,7 @@
     </row>
     <row r="12" spans="2:40" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="52" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C12" s="53">
         <v>7</v>
@@ -27994,7 +28010,7 @@
     </row>
     <row r="13" spans="2:40" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="52" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C13" s="53">
         <v>7</v>
@@ -28113,7 +28129,7 @@
     </row>
     <row r="14" spans="2:40" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="52" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C14" s="53">
         <v>9</v>
@@ -28232,7 +28248,7 @@
     </row>
     <row r="15" spans="2:40" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C15" s="1">
         <v>9</v>
@@ -28351,7 +28367,7 @@
     </row>
     <row r="16" spans="2:40" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C16" s="1">
         <v>10</v>
@@ -28470,7 +28486,7 @@
     </row>
     <row r="17" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B17" s="52" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C17" s="53">
         <v>10</v>
@@ -28589,7 +28605,7 @@
     </row>
     <row r="18" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C18" s="1">
         <v>11</v>
@@ -28708,7 +28724,7 @@
     </row>
     <row r="19" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B19" s="52" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C19" s="53">
         <v>12</v>
@@ -28827,7 +28843,7 @@
     </row>
     <row r="20" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B20" s="52" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C20" s="53">
         <v>13</v>
@@ -28946,7 +28962,7 @@
     </row>
     <row r="21" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C21" s="1">
         <v>14</v>
@@ -29065,7 +29081,7 @@
     </row>
     <row r="22" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B22" s="52" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C22" s="53">
         <v>15</v>
@@ -29769,7 +29785,7 @@
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="38" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
arreglo sincronizacion disponibilidades y crews base de datos - excel
</commit_message>
<xml_diff>
--- a/Backend/python/Datos_v8.xlsx
+++ b/Backend/python/Datos_v8.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="126">
   <si>
     <t>ID</t>
   </si>
@@ -118,10 +118,7 @@
     <t>Matias</t>
   </si>
   <si>
-    <t>asda</t>
-  </si>
-  <si>
-    <t>adsasddas</t>
+    <t>asdasdas</t>
   </si>
   <si>
     <t>Hora inicio bloque</t>
@@ -976,13 +973,13 @@
   <sheetData>
     <row r="1" ht="26.25" customHeight="1" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="C1" s="22" t="s">
         <v>46</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -1091,7 +1088,7 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
@@ -1115,7 +1112,7 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
@@ -1159,7 +1156,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="29"/>
       <c r="E13" s="21"/>
@@ -1178,18 +1175,18 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="C17" s="31" t="s">
         <v>52</v>
-      </c>
-      <c r="C17" s="31" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B18" s="33">
         <v>1</v>
@@ -1200,7 +1197,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B19" s="33">
         <v>2</v>
@@ -1211,7 +1208,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B20" s="33">
         <v>3</v>
@@ -1222,7 +1219,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B21" s="33">
         <v>4</v>
@@ -1233,7 +1230,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B22" s="33">
         <v>5</v>
@@ -1244,7 +1241,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" s="33">
         <v>6</v>
@@ -1255,7 +1252,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B24" s="33">
         <v>7</v>
@@ -1288,37 +1285,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -2546,16 +2543,16 @@
         <v>6</v>
       </c>
       <c r="K3" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L3" s="7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="M3" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N3" s="7">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -2575,16 +2572,16 @@
         <v>0</v>
       </c>
       <c r="H4" s="7">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I4" s="7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K4" s="7">
         <v>3</v>
       </c>
       <c r="L4" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M4" s="7">
         <v>3</v>
@@ -2610,16 +2607,16 @@
         <v>1</v>
       </c>
       <c r="H5" s="7">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I5" s="7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K5" s="7">
         <v>3</v>
       </c>
       <c r="L5" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M5" s="7">
         <v>3</v>
@@ -2654,7 +2651,7 @@
         <v>3</v>
       </c>
       <c r="L6" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M6" s="7">
         <v>3</v>
@@ -2689,7 +2686,7 @@
         <v>3</v>
       </c>
       <c r="L7" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M7" s="7">
         <v>3</v>
@@ -2724,7 +2721,7 @@
         <v>3</v>
       </c>
       <c r="L8" s="7">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="M8" s="7">
         <v>3</v>
@@ -2756,16 +2753,16 @@
         <v>5</v>
       </c>
       <c r="K9" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L9" s="7">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="M9" s="7">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="N9" s="7">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -2794,7 +2791,7 @@
         <v>4</v>
       </c>
       <c r="L10" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M10" s="7">
         <v>18</v>
@@ -2829,7 +2826,7 @@
         <v>4</v>
       </c>
       <c r="L11" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M11" s="7">
         <v>18</v>
@@ -2864,10 +2861,10 @@
         <v>4</v>
       </c>
       <c r="L12" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M12" s="7">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="N12" s="7">
         <v>32</v>
@@ -2899,7 +2896,7 @@
         <v>4</v>
       </c>
       <c r="L13" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M13" s="7">
         <v>18</v>
@@ -2931,13 +2928,13 @@
         <v>5</v>
       </c>
       <c r="K14" s="7">
+        <v>4</v>
+      </c>
+      <c r="L14" s="7">
         <v>5</v>
       </c>
-      <c r="L14" s="7">
-        <v>1</v>
-      </c>
       <c r="M14" s="7">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="N14" s="7">
         <v>32</v>
@@ -2969,7 +2966,7 @@
         <v>5</v>
       </c>
       <c r="L15" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M15" s="7">
         <v>18</v>
@@ -3004,7 +3001,7 @@
         <v>5</v>
       </c>
       <c r="L16" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M16" s="7">
         <v>18</v>
@@ -3039,10 +3036,10 @@
         <v>5</v>
       </c>
       <c r="L17" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M17" s="7">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="N17" s="7">
         <v>32</v>
@@ -3074,10 +3071,10 @@
         <v>5</v>
       </c>
       <c r="L18" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M18" s="7">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="N18" s="7">
         <v>32</v>
@@ -3112,7 +3109,7 @@
         <v>1</v>
       </c>
       <c r="M19" s="7">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N19" s="7">
         <v>32</v>
@@ -3126,13 +3123,13 @@
         <v>32</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D20" s="10">
         <v>0</v>
       </c>
       <c r="E20" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="1">
         <v>16</v>
@@ -3147,28 +3144,15 @@
         <v>2</v>
       </c>
       <c r="M20" s="7">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N20" s="7">
         <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="1">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
+      <c r="A21" s="1"/>
+      <c r="D21" s="1"/>
       <c r="H21" s="1">
         <v>16</v>
       </c>
@@ -3224,10 +3208,10 @@
         <v>9</v>
       </c>
       <c r="L23" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M23" s="7">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N23" s="7">
         <v>32</v>
@@ -3246,10 +3230,10 @@
         <v>9</v>
       </c>
       <c r="L24" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M24" s="7">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N24" s="7">
         <v>32</v>
@@ -3262,29 +3246,29 @@
         <v>18</v>
       </c>
       <c r="I25" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K25" s="7">
         <v>9</v>
       </c>
       <c r="L25" s="7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M25" s="7">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="N25" s="7">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="D26" s="1"/>
       <c r="H26" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I26" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K26" s="7">
         <v>10</v>
@@ -3293,7 +3277,7 @@
         <v>1</v>
       </c>
       <c r="M26" s="7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N26" s="7">
         <v>32</v>
@@ -3311,7 +3295,7 @@
         <v>2</v>
       </c>
       <c r="M27" s="7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N27" s="7">
         <v>32</v>
@@ -3329,7 +3313,7 @@
         <v>3</v>
       </c>
       <c r="M28" s="7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N28" s="7">
         <v>32</v>
@@ -3347,7 +3331,7 @@
         <v>4</v>
       </c>
       <c r="M29" s="7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N29" s="7">
         <v>32</v>
@@ -3365,7 +3349,7 @@
         <v>5</v>
       </c>
       <c r="M30" s="7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N30" s="7">
         <v>32</v>
@@ -3383,7 +3367,7 @@
         <v>6</v>
       </c>
       <c r="M31" s="7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N31" s="7">
         <v>32</v>
@@ -3401,7 +3385,7 @@
         <v>7</v>
       </c>
       <c r="M32" s="7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N32" s="7">
         <v>32</v>
@@ -3413,13 +3397,13 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="K33" s="7">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L33" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M33" s="7">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="N33" s="7">
         <v>32</v>
@@ -3431,13 +3415,13 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="K34" s="7">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L34" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M34" s="7">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="N34" s="7">
         <v>32</v>
@@ -3449,13 +3433,13 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="K35" s="7">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="L35" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M35" s="7">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="N35" s="7">
         <v>32</v>
@@ -3467,13 +3451,13 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="K36" s="1">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="L36" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="M36" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="N36" s="1">
         <v>32</v>
@@ -3485,13 +3469,13 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="K37" s="1">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="L37" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="M37" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="N37" s="1">
         <v>32</v>
@@ -3502,200 +3486,360 @@
       <c r="D38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-      <c r="N38" s="1"/>
+      <c r="K38" s="1">
+        <v>12</v>
+      </c>
+      <c r="L38" s="1">
+        <v>1</v>
+      </c>
+      <c r="M38" s="1">
+        <v>5</v>
+      </c>
+      <c r="N38" s="1">
+        <v>29</v>
+      </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="D39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
-      <c r="N39" s="1"/>
+      <c r="K39" s="1">
+        <v>12</v>
+      </c>
+      <c r="L39" s="1">
+        <v>2</v>
+      </c>
+      <c r="M39" s="1">
+        <v>5</v>
+      </c>
+      <c r="N39" s="1">
+        <v>29</v>
+      </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="D40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
-      <c r="N40" s="1"/>
+      <c r="K40" s="1">
+        <v>12</v>
+      </c>
+      <c r="L40" s="1">
+        <v>3</v>
+      </c>
+      <c r="M40" s="1">
+        <v>3</v>
+      </c>
+      <c r="N40" s="1">
+        <v>32</v>
+      </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="D41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
-      <c r="N41" s="1"/>
+      <c r="K41" s="1">
+        <v>12</v>
+      </c>
+      <c r="L41" s="1">
+        <v>4</v>
+      </c>
+      <c r="M41" s="1">
+        <v>3</v>
+      </c>
+      <c r="N41" s="1">
+        <v>32</v>
+      </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="D42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
+      <c r="K42" s="1">
+        <v>12</v>
+      </c>
+      <c r="L42" s="1">
+        <v>5</v>
+      </c>
+      <c r="M42" s="1">
+        <v>3</v>
+      </c>
+      <c r="N42" s="1">
+        <v>32</v>
+      </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="D43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
-      <c r="K43" s="1"/>
-      <c r="L43" s="1"/>
-      <c r="M43" s="1"/>
-      <c r="N43" s="1"/>
+      <c r="K43" s="1">
+        <v>12</v>
+      </c>
+      <c r="L43" s="1">
+        <v>6</v>
+      </c>
+      <c r="M43" s="1">
+        <v>3</v>
+      </c>
+      <c r="N43" s="1">
+        <v>32</v>
+      </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="D44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
-      <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
-      <c r="N44" s="1"/>
+      <c r="K44" s="1">
+        <v>12</v>
+      </c>
+      <c r="L44" s="1">
+        <v>7</v>
+      </c>
+      <c r="M44" s="1">
+        <v>3</v>
+      </c>
+      <c r="N44" s="1">
+        <v>32</v>
+      </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="D45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
-      <c r="K45" s="1"/>
-      <c r="L45" s="1"/>
-      <c r="M45" s="1"/>
-      <c r="N45" s="1"/>
+      <c r="K45" s="1">
+        <v>17</v>
+      </c>
+      <c r="L45" s="1">
+        <v>1</v>
+      </c>
+      <c r="M45" s="1">
+        <v>1</v>
+      </c>
+      <c r="N45" s="1">
+        <v>29</v>
+      </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="D46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
-      <c r="K46" s="1"/>
-      <c r="L46" s="1"/>
-      <c r="M46" s="1"/>
-      <c r="N46" s="1"/>
+      <c r="K46" s="1">
+        <v>17</v>
+      </c>
+      <c r="L46" s="1">
+        <v>2</v>
+      </c>
+      <c r="M46" s="1">
+        <v>1</v>
+      </c>
+      <c r="N46" s="1">
+        <v>29</v>
+      </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="D47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
-      <c r="K47" s="1"/>
-      <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
-      <c r="N47" s="1"/>
+      <c r="K47" s="1">
+        <v>17</v>
+      </c>
+      <c r="L47" s="1">
+        <v>3</v>
+      </c>
+      <c r="M47" s="1">
+        <v>1</v>
+      </c>
+      <c r="N47" s="1">
+        <v>29</v>
+      </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="D48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
-      <c r="K48" s="1"/>
-      <c r="L48" s="1"/>
-      <c r="M48" s="1"/>
-      <c r="N48" s="1"/>
+      <c r="K48" s="1">
+        <v>17</v>
+      </c>
+      <c r="L48" s="1">
+        <v>4</v>
+      </c>
+      <c r="M48" s="1">
+        <v>1</v>
+      </c>
+      <c r="N48" s="1">
+        <v>29</v>
+      </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="D49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
-      <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
+      <c r="K49" s="1">
+        <v>17</v>
+      </c>
+      <c r="L49" s="1">
+        <v>5</v>
+      </c>
+      <c r="M49" s="1">
+        <v>1</v>
+      </c>
+      <c r="N49" s="1">
+        <v>29</v>
+      </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="D50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
-      <c r="K50" s="1"/>
-      <c r="L50" s="1"/>
-      <c r="M50" s="1"/>
-      <c r="N50" s="1"/>
+      <c r="K50" s="1">
+        <v>17</v>
+      </c>
+      <c r="L50" s="1">
+        <v>6</v>
+      </c>
+      <c r="M50" s="1">
+        <v>1</v>
+      </c>
+      <c r="N50" s="1">
+        <v>29</v>
+      </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="D51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
-      <c r="K51" s="1"/>
-      <c r="L51" s="1"/>
-      <c r="M51" s="1"/>
-      <c r="N51" s="1"/>
+      <c r="K51" s="1">
+        <v>17</v>
+      </c>
+      <c r="L51" s="1">
+        <v>7</v>
+      </c>
+      <c r="M51" s="1">
+        <v>1</v>
+      </c>
+      <c r="N51" s="1">
+        <v>29</v>
+      </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="D52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
-      <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
+      <c r="K52" s="1">
+        <v>18</v>
+      </c>
+      <c r="L52" s="1">
+        <v>4</v>
+      </c>
+      <c r="M52" s="1">
+        <v>7</v>
+      </c>
+      <c r="N52" s="1">
+        <v>29</v>
+      </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="D53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
-      <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
+      <c r="K53" s="1">
+        <v>18</v>
+      </c>
+      <c r="L53" s="1">
+        <v>5</v>
+      </c>
+      <c r="M53" s="1">
+        <v>1</v>
+      </c>
+      <c r="N53" s="1">
+        <v>29</v>
+      </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="D54" s="1"/>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
-      <c r="K54" s="1"/>
-      <c r="L54" s="1"/>
-      <c r="M54" s="1"/>
-      <c r="N54" s="1"/>
+      <c r="K54" s="1">
+        <v>19</v>
+      </c>
+      <c r="L54" s="1">
+        <v>1</v>
+      </c>
+      <c r="M54" s="1">
+        <v>3</v>
+      </c>
+      <c r="N54" s="1">
+        <v>24</v>
+      </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="D55" s="1"/>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
-      <c r="K55" s="1"/>
-      <c r="L55" s="1"/>
-      <c r="M55" s="1"/>
-      <c r="N55" s="1"/>
+      <c r="K55" s="1">
+        <v>19</v>
+      </c>
+      <c r="L55" s="1">
+        <v>2</v>
+      </c>
+      <c r="M55" s="1">
+        <v>1</v>
+      </c>
+      <c r="N55" s="1">
+        <v>24</v>
+      </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="D56" s="1"/>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
-      <c r="K56" s="1"/>
-      <c r="L56" s="1"/>
-      <c r="M56" s="1"/>
-      <c r="N56" s="1"/>
+      <c r="K56" s="1">
+        <v>19</v>
+      </c>
+      <c r="L56" s="1">
+        <v>4</v>
+      </c>
+      <c r="M56" s="1">
+        <v>3</v>
+      </c>
+      <c r="N56" s="1">
+        <v>32</v>
+      </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="D57" s="1"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
-      <c r="K57" s="1"/>
-      <c r="L57" s="1"/>
-      <c r="M57" s="1"/>
-      <c r="N57" s="1"/>
+      <c r="K57" s="1">
+        <v>19</v>
+      </c>
+      <c r="L57" s="1">
+        <v>7</v>
+      </c>
+      <c r="M57" s="1">
+        <v>3</v>
+      </c>
+      <c r="N57" s="1">
+        <v>32</v>
+      </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
@@ -19564,25 +19708,25 @@
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="I2" s="35">
         <v>0.3333333333321207</v>
@@ -19684,7 +19828,7 @@
     <row r="3" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -19804,7 +19948,7 @@
     <row r="4" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
@@ -19924,7 +20068,7 @@
     <row r="5" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
@@ -20044,7 +20188,7 @@
     <row r="6" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" s="1">
         <v>5</v>
@@ -20164,7 +20308,7 @@
     <row r="7" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C7" s="1">
         <v>7</v>
@@ -20284,7 +20428,7 @@
     <row r="8" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C8" s="1">
         <v>9</v>
@@ -20404,7 +20548,7 @@
     <row r="9" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C9" s="1">
         <v>12</v>
@@ -21113,7 +21257,7 @@
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -21148,25 +21292,25 @@
         <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="I2" s="35">
         <v>0.3333333333321207</v>
@@ -21268,7 +21412,7 @@
     <row r="3" spans="1:40" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="44"/>
       <c r="B3" s="45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="46">
         <v>2</v>
@@ -21388,7 +21532,7 @@
     <row r="4" spans="1:40" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="44"/>
       <c r="B4" s="45" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="46">
         <v>2</v>
@@ -21508,7 +21652,7 @@
     <row r="5" spans="1:40" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="44"/>
       <c r="B5" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="10">
         <v>3</v>
@@ -21628,7 +21772,7 @@
     <row r="6" spans="1:40" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="44"/>
       <c r="B6" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="10">
         <v>5</v>
@@ -21748,7 +21892,7 @@
     <row r="7" spans="1:40" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="44"/>
       <c r="B7" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C7" s="10">
         <v>7</v>
@@ -21867,7 +22011,7 @@
     </row>
     <row r="8" spans="2:40" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C8" s="46">
         <v>9</v>
@@ -21987,7 +22131,7 @@
     <row r="9" spans="1:40" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="44"/>
       <c r="B9" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C9" s="10">
         <v>9</v>
@@ -22106,7 +22250,7 @@
     </row>
     <row r="10" spans="2:40" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" s="46">
         <v>11</v>
@@ -22226,7 +22370,7 @@
     <row r="11" spans="1:40" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="44"/>
       <c r="B11" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C11" s="10">
         <v>11</v>
@@ -22346,7 +22490,7 @@
     <row r="12" spans="1:40" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="44"/>
       <c r="B12" s="45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C12" s="46">
         <v>11</v>
@@ -22466,7 +22610,7 @@
     <row r="13" spans="1:40" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="44"/>
       <c r="B13" s="45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C13" s="46">
         <v>13</v>
@@ -22586,7 +22730,7 @@
     <row r="14" spans="1:41" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="44"/>
       <c r="B14" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C14" s="10">
         <v>13</v>
@@ -22707,7 +22851,7 @@
     <row r="15" spans="1:41" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="44"/>
       <c r="B15" s="45" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C15" s="46">
         <v>14</v>
@@ -22828,7 +22972,7 @@
     <row r="16" spans="1:40" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="51"/>
       <c r="B16" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C16" s="10">
         <v>14</v>
@@ -22948,7 +23092,7 @@
     <row r="17" spans="1:40" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="51"/>
       <c r="B17" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C17" s="10">
         <v>15</v>
@@ -23068,7 +23212,7 @@
     <row r="18" spans="1:40" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="51"/>
       <c r="B18" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C18" s="10">
         <v>18</v>
@@ -23188,7 +23332,7 @@
     <row r="19" spans="1:40" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="51"/>
       <c r="B19" s="45" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C19" s="46">
         <v>20</v>
@@ -24248,7 +24392,7 @@
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -24283,25 +24427,25 @@
         <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="I2" s="35">
         <v>0.3333333333321207</v>
@@ -24403,7 +24547,7 @@
     <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" s="34"/>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" s="1">
         <v>5</v>
@@ -24523,7 +24667,7 @@
     <row r="4" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="52" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" s="53">
         <v>5</v>
@@ -24643,7 +24787,7 @@
     <row r="5" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C5" s="1">
         <v>7</v>
@@ -24763,7 +24907,7 @@
     <row r="6" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C6" s="1">
         <v>9</v>
@@ -24883,7 +25027,7 @@
     <row r="7" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C7" s="1">
         <v>11</v>
@@ -25003,7 +25147,7 @@
     <row r="8" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="52" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C8" s="53">
         <v>13</v>
@@ -25123,7 +25267,7 @@
     <row r="9" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="52" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C9" s="53">
         <v>14</v>
@@ -25243,7 +25387,7 @@
     <row r="10" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C10" s="1">
         <v>13</v>
@@ -25363,7 +25507,7 @@
     <row r="11" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C11" s="1">
         <v>14</v>
@@ -25483,7 +25627,7 @@
     <row r="12" spans="1:40" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="39"/>
       <c r="B12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C12" s="1">
         <v>15</v>
@@ -25603,7 +25747,7 @@
     <row r="13" spans="1:40" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="39"/>
       <c r="B13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C13" s="1">
         <v>17</v>
@@ -25723,7 +25867,7 @@
     <row r="14" spans="1:40" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="39"/>
       <c r="B14" s="52" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C14" s="53">
         <v>18</v>
@@ -25843,7 +25987,7 @@
     <row r="15" spans="1:40" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="39"/>
       <c r="B15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C15" s="1">
         <v>20</v>
@@ -26666,7 +26810,7 @@
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -26701,25 +26845,25 @@
         <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="I2" s="35">
         <v>0.3333333333321207</v>
@@ -26820,7 +26964,7 @@
     </row>
     <row r="3" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -26939,7 +27083,7 @@
     </row>
     <row r="4" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B4" s="52" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C4" s="53">
         <v>1</v>
@@ -27058,7 +27202,7 @@
     </row>
     <row r="5" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
@@ -27177,7 +27321,7 @@
     </row>
     <row r="6" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B6" s="52" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C6" s="53">
         <v>2</v>
@@ -27296,7 +27440,7 @@
     </row>
     <row r="7" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B7" s="52" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C7" s="53">
         <v>3</v>
@@ -27415,7 +27559,7 @@
     </row>
     <row r="8" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C8" s="1">
         <v>3</v>
@@ -27534,7 +27678,7 @@
     </row>
     <row r="9" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B9" s="52" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C9" s="53">
         <v>5</v>
@@ -27653,7 +27797,7 @@
     </row>
     <row r="10" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C10" s="1">
         <v>5</v>
@@ -27772,7 +27916,7 @@
     </row>
     <row r="11" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C11" s="1">
         <v>7</v>
@@ -27891,7 +28035,7 @@
     </row>
     <row r="12" spans="2:40" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="52" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C12" s="53">
         <v>7</v>
@@ -28010,7 +28154,7 @@
     </row>
     <row r="13" spans="2:40" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="52" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C13" s="53">
         <v>7</v>
@@ -28129,7 +28273,7 @@
     </row>
     <row r="14" spans="2:40" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="52" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C14" s="53">
         <v>9</v>
@@ -28248,7 +28392,7 @@
     </row>
     <row r="15" spans="2:40" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C15" s="1">
         <v>9</v>
@@ -28367,7 +28511,7 @@
     </row>
     <row r="16" spans="2:40" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C16" s="1">
         <v>10</v>
@@ -28486,7 +28630,7 @@
     </row>
     <row r="17" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B17" s="52" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C17" s="53">
         <v>10</v>
@@ -28605,7 +28749,7 @@
     </row>
     <row r="18" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C18" s="1">
         <v>11</v>
@@ -28724,7 +28868,7 @@
     </row>
     <row r="19" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B19" s="52" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C19" s="53">
         <v>12</v>
@@ -28843,7 +28987,7 @@
     </row>
     <row r="20" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B20" s="52" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C20" s="53">
         <v>13</v>
@@ -28962,7 +29106,7 @@
     </row>
     <row r="21" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C21" s="1">
         <v>14</v>
@@ -29081,7 +29225,7 @@
     </row>
     <row r="22" spans="2:40" x14ac:dyDescent="0.25">
       <c r="B22" s="52" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C22" s="53">
         <v>15</v>
@@ -29785,7 +29929,7 @@
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
arreglo en intercambio de turnos con swaps triviales
</commit_message>
<xml_diff>
--- a/Backend/python/Datos_v8.xlsx
+++ b/Backend/python/Datos_v8.xlsx
@@ -2543,16 +2543,16 @@
         <v>6</v>
       </c>
       <c r="K3" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L3" s="7">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="M3" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N3" s="7">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -2581,7 +2581,7 @@
         <v>3</v>
       </c>
       <c r="L4" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M4" s="7">
         <v>3</v>
@@ -2616,7 +2616,7 @@
         <v>3</v>
       </c>
       <c r="L5" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M5" s="7">
         <v>3</v>
@@ -2651,7 +2651,7 @@
         <v>3</v>
       </c>
       <c r="L6" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M6" s="7">
         <v>3</v>
@@ -2686,7 +2686,7 @@
         <v>3</v>
       </c>
       <c r="L7" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M7" s="7">
         <v>3</v>
@@ -2721,7 +2721,7 @@
         <v>3</v>
       </c>
       <c r="L8" s="7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="M8" s="7">
         <v>3</v>
@@ -2753,16 +2753,16 @@
         <v>5</v>
       </c>
       <c r="K9" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L9" s="7">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="M9" s="7">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="N9" s="7">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -2791,7 +2791,7 @@
         <v>4</v>
       </c>
       <c r="L10" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M10" s="7">
         <v>18</v>
@@ -2826,7 +2826,7 @@
         <v>4</v>
       </c>
       <c r="L11" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M11" s="7">
         <v>18</v>
@@ -2861,7 +2861,7 @@
         <v>4</v>
       </c>
       <c r="L12" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M12" s="7">
         <v>18</v>
@@ -2896,10 +2896,10 @@
         <v>4</v>
       </c>
       <c r="L13" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M13" s="7">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="N13" s="7">
         <v>32</v>
@@ -2928,13 +2928,13 @@
         <v>5</v>
       </c>
       <c r="K14" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L14" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M14" s="7">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="N14" s="7">
         <v>32</v>
@@ -2966,7 +2966,7 @@
         <v>5</v>
       </c>
       <c r="L15" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M15" s="7">
         <v>18</v>
@@ -3001,7 +3001,7 @@
         <v>5</v>
       </c>
       <c r="L16" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M16" s="7">
         <v>18</v>
@@ -3036,10 +3036,10 @@
         <v>5</v>
       </c>
       <c r="L17" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M17" s="7">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="N17" s="7">
         <v>32</v>
@@ -3068,13 +3068,13 @@
         <v>4</v>
       </c>
       <c r="K18" s="7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L18" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M18" s="7">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N18" s="7">
         <v>32</v>
@@ -3106,7 +3106,7 @@
         <v>7</v>
       </c>
       <c r="L19" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M19" s="7">
         <v>14</v>
@@ -3141,10 +3141,10 @@
         <v>7</v>
       </c>
       <c r="L20" s="7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M20" s="7">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="N20" s="7">
         <v>32</v>
@@ -3163,7 +3163,7 @@
         <v>7</v>
       </c>
       <c r="L21" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M21" s="7">
         <v>18</v>
@@ -3183,13 +3183,13 @@
         <v>3</v>
       </c>
       <c r="K22" s="7">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="L22" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M22" s="7">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="N22" s="7">
         <v>32</v>
@@ -3208,7 +3208,7 @@
         <v>9</v>
       </c>
       <c r="L23" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M23" s="7">
         <v>15</v>
@@ -3230,10 +3230,10 @@
         <v>9</v>
       </c>
       <c r="L24" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M24" s="7">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="N24" s="7">
         <v>32</v>
@@ -3249,13 +3249,13 @@
         <v>3</v>
       </c>
       <c r="K25" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L25" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M25" s="7">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="N25" s="7">
         <v>32</v>
@@ -3274,7 +3274,7 @@
         <v>10</v>
       </c>
       <c r="L26" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M26" s="7">
         <v>7</v>
@@ -3292,7 +3292,7 @@
         <v>10</v>
       </c>
       <c r="L27" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M27" s="7">
         <v>7</v>
@@ -3310,7 +3310,7 @@
         <v>10</v>
       </c>
       <c r="L28" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M28" s="7">
         <v>7</v>
@@ -3328,7 +3328,7 @@
         <v>10</v>
       </c>
       <c r="L29" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M29" s="7">
         <v>7</v>
@@ -3346,7 +3346,7 @@
         <v>10</v>
       </c>
       <c r="L30" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M30" s="7">
         <v>7</v>
@@ -3364,7 +3364,7 @@
         <v>10</v>
       </c>
       <c r="L31" s="7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M31" s="7">
         <v>7</v>
@@ -3379,13 +3379,13 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="K32" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L32" s="7">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="M32" s="7">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="N32" s="7">
         <v>32</v>
@@ -3400,7 +3400,7 @@
         <v>11</v>
       </c>
       <c r="L33" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M33" s="7">
         <v>3</v>
@@ -3418,7 +3418,7 @@
         <v>11</v>
       </c>
       <c r="L34" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M34" s="7">
         <v>3</v>
@@ -3436,7 +3436,7 @@
         <v>11</v>
       </c>
       <c r="L35" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M35" s="7">
         <v>3</v>
@@ -3454,7 +3454,7 @@
         <v>11</v>
       </c>
       <c r="L36" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M36" s="1">
         <v>3</v>
@@ -3469,16 +3469,16 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="K37" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L37" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="M37" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N37" s="1">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -3490,7 +3490,7 @@
         <v>12</v>
       </c>
       <c r="L38" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M38" s="1">
         <v>5</v>
@@ -3508,13 +3508,13 @@
         <v>12</v>
       </c>
       <c r="L39" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M39" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N39" s="1">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
@@ -3526,7 +3526,7 @@
         <v>12</v>
       </c>
       <c r="L40" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M40" s="1">
         <v>3</v>
@@ -3544,7 +3544,7 @@
         <v>12</v>
       </c>
       <c r="L41" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M41" s="1">
         <v>3</v>
@@ -3562,7 +3562,7 @@
         <v>12</v>
       </c>
       <c r="L42" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M42" s="1">
         <v>3</v>
@@ -3580,7 +3580,7 @@
         <v>12</v>
       </c>
       <c r="L43" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M43" s="1">
         <v>3</v>
@@ -3595,16 +3595,16 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="K44" s="1">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="L44" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="M44" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N44" s="1">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
@@ -3616,7 +3616,7 @@
         <v>17</v>
       </c>
       <c r="L45" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M45" s="1">
         <v>1</v>
@@ -3634,7 +3634,7 @@
         <v>17</v>
       </c>
       <c r="L46" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M46" s="1">
         <v>1</v>
@@ -3652,7 +3652,7 @@
         <v>17</v>
       </c>
       <c r="L47" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M47" s="1">
         <v>1</v>
@@ -3670,7 +3670,7 @@
         <v>17</v>
       </c>
       <c r="L48" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M48" s="1">
         <v>1</v>
@@ -3688,7 +3688,7 @@
         <v>17</v>
       </c>
       <c r="L49" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M49" s="1">
         <v>1</v>
@@ -3706,7 +3706,7 @@
         <v>17</v>
       </c>
       <c r="L50" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M50" s="1">
         <v>1</v>
@@ -3721,13 +3721,13 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="K51" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L51" s="1">
+        <v>4</v>
+      </c>
+      <c r="M51" s="1">
         <v>7</v>
-      </c>
-      <c r="M51" s="1">
-        <v>1</v>
       </c>
       <c r="N51" s="1">
         <v>29</v>
@@ -3742,10 +3742,10 @@
         <v>18</v>
       </c>
       <c r="L52" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M52" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="N52" s="1">
         <v>29</v>
@@ -3757,16 +3757,16 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
       <c r="K53" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L53" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M53" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N53" s="1">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
@@ -3778,10 +3778,10 @@
         <v>19</v>
       </c>
       <c r="L54" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M54" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N54" s="1">
         <v>24</v>
@@ -3796,13 +3796,13 @@
         <v>19</v>
       </c>
       <c r="L55" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M55" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N55" s="1">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
@@ -3814,7 +3814,7 @@
         <v>19</v>
       </c>
       <c r="L56" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="M56" s="1">
         <v>3</v>
@@ -3828,18 +3828,10 @@
       <c r="D57" s="1"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
-      <c r="K57" s="1">
-        <v>19</v>
-      </c>
-      <c r="L57" s="1">
-        <v>7</v>
-      </c>
-      <c r="M57" s="1">
-        <v>3</v>
-      </c>
-      <c r="N57" s="1">
-        <v>32</v>
-      </c>
+      <c r="K57" s="1"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>

</xml_diff>

<commit_message>
correción generar turnos automaticos en planilla manual, y estilos en general con respecto al fondo
</commit_message>
<xml_diff>
--- a/Backend/python/Datos_v8.xlsx
+++ b/Backend/python/Datos_v8.xlsx
@@ -2569,7 +2569,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="7">
         <v>7</v>
@@ -3059,7 +3059,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" s="1">
         <v>15</v>
@@ -3094,7 +3094,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" s="1">
         <v>15</v>

</xml_diff>

<commit_message>
ajuste para tener en consideracion los beneficios para los horarios automaticos
</commit_message>
<xml_diff>
--- a/Backend/python/Datos_v8.xlsx
+++ b/Backend/python/Datos_v8.xlsx
@@ -14083,60 +14083,30 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="M12" s="11"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>18</v>
-      </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>18</v>
-      </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>18</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="C15">
-        <v>5</v>
-      </c>
-    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Implementación de intercambios de turnos en planilla de turnos.
</commit_message>
<xml_diff>
--- a/Backend/python/Datos_v8.xlsx
+++ b/Backend/python/Datos_v8.xlsx
@@ -3603,7 +3603,7 @@
         <v>17</v>
       </c>
       <c r="L45" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M45" s="1">
         <v>1</v>
@@ -3621,7 +3621,7 @@
         <v>17</v>
       </c>
       <c r="L46" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M46" s="1">
         <v>1</v>
@@ -3639,7 +3639,7 @@
         <v>17</v>
       </c>
       <c r="L47" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M47" s="1">
         <v>1</v>
@@ -3657,7 +3657,7 @@
         <v>17</v>
       </c>
       <c r="L48" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M48" s="1">
         <v>1</v>
@@ -3675,7 +3675,7 @@
         <v>17</v>
       </c>
       <c r="L49" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M49" s="1">
         <v>1</v>
@@ -3690,13 +3690,13 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
       <c r="K50" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L50" s="1">
+        <v>4</v>
+      </c>
+      <c r="M50" s="1">
         <v>7</v>
-      </c>
-      <c r="M50" s="1">
-        <v>1</v>
       </c>
       <c r="N50" s="1">
         <v>29</v>
@@ -3711,10 +3711,10 @@
         <v>18</v>
       </c>
       <c r="L51" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M51" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="N51" s="1">
         <v>29</v>
@@ -3725,18 +3725,10 @@
       <c r="D52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
-      <c r="K52" s="1">
-        <v>18</v>
-      </c>
-      <c r="L52" s="1">
-        <v>5</v>
-      </c>
-      <c r="M52" s="1">
-        <v>1</v>
-      </c>
-      <c r="N52" s="1">
-        <v>29</v>
-      </c>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
@@ -29886,7 +29878,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M200"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="E21" sqref="E21"/>
@@ -29916,206 +29908,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M12" s="11"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
estandarización de apis en frontend
</commit_message>
<xml_diff>
--- a/Backend/python/Datos_v8.xlsx
+++ b/Backend/python/Datos_v8.xlsx
@@ -29878,7 +29878,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M200"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="E21" sqref="E21"/>
@@ -29897,20 +29897,207 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M12" s="11"/>
     </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>